<commit_message>
April 6, 2020 Commits
</commit_message>
<xml_diff>
--- a/export_rfq.xlsx
+++ b/export_rfq.xlsx
@@ -46,7 +46,7 @@
     <t>RFQ Number :</t>
   </si>
   <si>
-    <t>2020-0090</t>
+    <t>2020-0094</t>
   </si>
   <si>
     <t>Mode of Procurement:</t>
@@ -55,7 +55,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>March 13,   2020</t>
+    <t>April 06,   2020</t>
   </si>
   <si>
     <t>Office/End User:</t>
@@ -67,7 +67,7 @@
     <t>Purpose:</t>
   </si>
   <si>
-    <t xml:space="preserve">Meals for HRMPSB Meeting </t>
+    <t xml:space="preserve">Test </t>
   </si>
   <si>
     <t>Company Name:</t>
@@ -169,9 +169,6 @@
     <t>Approved Budget for the Contract (ABC):</t>
   </si>
   <si>
-    <t>5,100.00</t>
-  </si>
-  <si>
     <t>DR. CARINA S. CRUZ</t>
   </si>
   <si>
@@ -226,11 +223,11 @@
     <t>NO</t>
   </si>
   <si>
-    <t xml:space="preserve">HRMPSB Meeting
+    <t xml:space="preserve">Copy Paper, A4, 80gsm, 500sheets
 </t>
   </si>
   <si>
-    <t>unit</t>
+    <t>ream</t>
   </si>
   <si>
     <t>REF:  approved and funded PPMP; approved and funded Activity Design	
@@ -238,6 +235,14 @@
 1. PhilGEPS Platinum Registration No. 									
 2. For non-Platinum Registration, please provide copy of:
     a) Mayor's Permit; b) Latest Income / Business Tax Return; c) PhilGEPS Registration No. _____________________________________									
+Other Instruction:</t>
+  </si>
+  <si>
+    <t>NOTE: ** A guaranteed of a minimum of 75% out of total number of target participants	
+              ** Free Flowing Coffee 
+              ** Free Wi-Fi
+              ** Atleast Triple/Quad Sharing Per Room  
+              ** Free use of Function Room, Sound System and LCD
 Other Instruction:</t>
   </si>
   <si>
@@ -2250,8 +2255,8 @@
       <c r="B38" s="112"/>
       <c r="C38" s="112"/>
       <c r="D38" s="112"/>
-      <c r="E38" s="113" t="s">
-        <v>45</v>
+      <c r="E38" s="113">
+        <v>350</v>
       </c>
       <c r="F38" s="113"/>
       <c r="G38" s="113"/>
@@ -2291,7 +2296,7 @@
       <c r="I40" s="89"/>
       <c r="J40" s="89"/>
       <c r="K40" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L40" s="18"/>
       <c r="M40" s="18"/>
@@ -2308,7 +2313,7 @@
       <c r="H41" s="113"/>
       <c r="I41" s="90"/>
       <c r="J41" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K41" s="19"/>
       <c r="L41" s="19"/>
@@ -2333,24 +2338,24 @@
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="14.25">
       <c r="A43" s="112" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" s="116" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="117"/>
       <c r="D43" s="118"/>
       <c r="E43" s="115" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="112" t="s">
         <v>50</v>
       </c>
-      <c r="F43" s="112" t="s">
+      <c r="G43" s="130" t="s">
         <v>51</v>
       </c>
-      <c r="G43" s="130" t="s">
+      <c r="H43" s="128" t="s">
         <v>52</v>
-      </c>
-      <c r="H43" s="128" t="s">
-        <v>53</v>
       </c>
       <c r="I43" s="128"/>
       <c r="J43" s="128"/>
@@ -2368,16 +2373,16 @@
       <c r="F44" s="112"/>
       <c r="G44" s="130"/>
       <c r="H44" s="126" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I44" s="127"/>
       <c r="J44" s="127"/>
       <c r="K44" s="125" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L44" s="125"/>
       <c r="M44" s="131" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N44" s="132"/>
     </row>
@@ -2438,19 +2443,19 @@
       <c r="F48" s="112"/>
       <c r="G48" s="130"/>
       <c r="H48" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="I48" s="139" t="s">
         <v>57</v>
       </c>
-      <c r="I48" s="139" t="s">
+      <c r="J48" s="141" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="141" t="s">
+      <c r="K48" s="143" t="s">
         <v>59</v>
       </c>
-      <c r="K48" s="143" t="s">
+      <c r="L48" s="144" t="s">
         <v>60</v>
-      </c>
-      <c r="L48" s="144" t="s">
-        <v>61</v>
       </c>
       <c r="M48" s="133"/>
       <c r="N48" s="134"/>
@@ -2474,18 +2479,18 @@
     <row r="50" spans="1:14">
       <c r="A50" s="145"/>
       <c r="B50" s="147" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="146"/>
       <c r="D50" s="146"/>
       <c r="E50" s="149">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F50" s="150" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G50" s="152">
-        <v>425</v>
+        <v>350</v>
       </c>
       <c r="H50" s="149"/>
       <c r="I50" s="152"/>
@@ -2497,7 +2502,7 @@
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="158" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" s="153"/>
       <c r="C51" s="153"/>
@@ -2515,7 +2520,7 @@
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="157" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B52" s="153"/>
       <c r="C52" s="153"/>
@@ -2533,7 +2538,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="157" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B53" s="153"/>
       <c r="C53" s="153"/>
@@ -2550,9 +2555,7 @@
       <c r="N53" s="156"/>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="157" t="s">
-        <v>65</v>
-      </c>
+      <c r="A54" s="157"/>
       <c r="B54" s="153"/>
       <c r="C54" s="153"/>
       <c r="D54" s="153"/>

</xml_diff>